<commit_message>
fix: removed duplicated lines
</commit_message>
<xml_diff>
--- a/LICENSES.xlsx
+++ b/LICENSES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\GitHub\Shawee\abrate-codigo-datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB58D63-31BF-4685-BC3C-9229E948CAC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3E817C-41E3-4652-8B28-4AA0CE81104C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t>Museu de Arte Contemporânea da Universidade de São Paulo</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>MUSEU DE ASTRONOMIA E CIÊNCIAS AFINS</t>
-  </si>
-  <si>
-    <t>MUSEU DE ASTRONOMIA E CIÊNCIAS AFINS (II)</t>
   </si>
   <si>
     <t>Arquivo</t>
@@ -440,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,10 +451,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -465,7 +462,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -473,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -481,7 +478,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -489,7 +486,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -497,7 +494,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -505,7 +502,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -513,7 +510,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -521,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -529,7 +526,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -537,7 +534,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -545,7 +542,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -553,7 +550,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -561,7 +558,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -569,7 +566,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -577,7 +574,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -585,7 +582,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -593,7 +590,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -601,7 +598,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -609,7 +606,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -617,31 +614,15 @@
         <v>12</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: removed duplicated lines
</commit_message>
<xml_diff>
--- a/LICENSES.xlsx
+++ b/LICENSES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\GitHub\Shawee\abrate-codigo-datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3E817C-41E3-4652-8B28-4AA0CE81104C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E677D34-11ED-474E-BC43-2D79DB29DEDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Museu de Arte Contemporânea da Universidade de São Paulo</t>
   </si>
@@ -437,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +483,7 @@
     </row>
     <row r="5" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="6" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="7" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>16</v>
@@ -507,39 +507,39 @@
     </row>
     <row r="8" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>16</v>
@@ -547,81 +547,25 @@
     </row>
     <row r="13" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>